<commit_message>
update example project to match new version directexcel plugin
</commit_message>
<xml_diff>
--- a/Tables/GameData.xlsx
+++ b/Tables/GameData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7D2635B4-41A9-4298-87D3-33460BDE4D44}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{57853548-41DF-4AF6-A18B-0B38AA1E5859}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,7 +362,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,13 +391,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>